<commit_message>
Revise, extend and clarify metadata
</commit_message>
<xml_diff>
--- a/Data/PWD_Remediation/CSO-002_and_CSO-004_Annual_Overflow_Volumes.xlsx
+++ b/Data/PWD_Remediation/CSO-002_and_CSO-004_Annual_Overflow_Volumes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9D0605-49A7-4528-A4D2-B2FB034EE9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>CSO-002 Warren Avenue</t>
   </si>
   <si>
     <t>CSO-004 Dunn Street</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,9 +101,9 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,192 +380,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>2005</v>
       </c>
+      <c r="B2" s="3">
+        <v>7138000</v>
+      </c>
       <c r="C2" s="3">
-        <v>7138000</v>
-      </c>
-      <c r="D2" s="3">
         <v>1075000</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2006</v>
       </c>
+      <c r="B3" s="3">
+        <v>6572033.1560221193</v>
+      </c>
       <c r="C3" s="3">
-        <v>6572033.1560221193</v>
-      </c>
-      <c r="D3" s="3">
         <v>3621443.3275610064</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2007</v>
       </c>
+      <c r="B4" s="3">
+        <v>4544369.2800000021</v>
+      </c>
       <c r="C4" s="3">
-        <v>4544369.2800000021</v>
-      </c>
-      <c r="D4" s="3">
         <v>5570864.6399999997</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>2008</v>
       </c>
+      <c r="B5" s="3">
+        <v>2099534</v>
+      </c>
       <c r="C5" s="3">
-        <v>2099534</v>
-      </c>
-      <c r="D5" s="3">
         <v>1364606</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>2009</v>
       </c>
+      <c r="B6" s="3">
+        <v>1136608</v>
+      </c>
       <c r="C6" s="3">
-        <v>1136608</v>
-      </c>
-      <c r="D6" s="3">
         <v>1371674</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>2010</v>
       </c>
+      <c r="B7" s="3">
+        <v>534000</v>
+      </c>
       <c r="C7" s="3">
-        <v>534000</v>
-      </c>
-      <c r="D7" s="3">
         <v>474597</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>2011</v>
       </c>
+      <c r="B8" s="3">
+        <v>3570000</v>
+      </c>
       <c r="C8" s="3">
-        <v>3570000</v>
-      </c>
-      <c r="D8" s="3">
         <v>1486000</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>2012</v>
       </c>
+      <c r="B9" s="3">
+        <v>5826000</v>
+      </c>
       <c r="C9" s="3">
-        <v>5826000</v>
-      </c>
-      <c r="D9" s="3">
         <v>1223000</v>
       </c>
+      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>2013</v>
       </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
       <c r="C10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>2014</v>
       </c>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
       <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
         <v>1140000</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>2015</v>
       </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
       <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3">
         <v>77000</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>2016</v>
       </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
         <v>78100</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>2017</v>
       </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
         <v>4000</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>2018</v>
       </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
       <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>2019</v>
       </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
       <c r="C16" s="3">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3">
         <v>147000</v>
       </c>
     </row>

</xml_diff>